<commit_message>
Sample coding scheme for Tutorial
</commit_message>
<xml_diff>
--- a/MyCodingScheme.xlsx
+++ b/MyCodingScheme.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="41880" yWindow="2780" windowWidth="28800" windowHeight="15900" tabRatio="500"/>
+    <workbookView xWindow="3780" yWindow="2980" windowWidth="28800" windowHeight="15900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="84">
   <si>
     <t>Scheme</t>
   </si>
@@ -229,6 +229,48 @@
   </si>
   <si>
     <t>junior member</t>
+  </si>
+  <si>
+    <t>assocId</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>enemyOf</t>
+  </si>
+  <si>
+    <t>enemyOF</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -598,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1066,48 +1108,45 @@
       <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="1" t="s">
-        <v>10</v>
+      <c r="A47" t="s">
+        <v>70</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>61</v>
@@ -1127,53 +1166,51 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C54" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1181,30 +1218,28 @@
         <v>64</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1218,92 +1253,210 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
+      <c r="A71" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="A72" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
+      <c r="A73" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="B75" s="1"/>
+      <c r="A75" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+      <c r="A76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="77" spans="1:3">
+      <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
     <row r="78" spans="1:3">
+      <c r="A78" s="1"/>
       <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
     </row>
     <row r="79" spans="1:3">
+      <c r="A79" s="1"/>
       <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:3">
+      <c r="A80" s="1"/>
       <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="B90" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Adding a sheet defining mapping to LexEVS/LexGrid
</commit_message>
<xml_diff>
--- a/MyCodingScheme.xlsx
+++ b/MyCodingScheme.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="2980" windowWidth="28800" windowHeight="15900" tabRatio="500"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21800" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -18,15 +19,118 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Scott Bauer</author>
+  </authors>
+  <commentList>
+    <comment ref="F11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Scott Bauer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+any generic property name needs to be declared here</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Scott Bauer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+add the source element of same name associations.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Scott Bauer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+No curated propertyName so we create our own.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Scott Bauer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+We have no other namespaces declared so the enclosing coding scheme suffices.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="110">
   <si>
     <t>Scheme</t>
   </si>
   <si>
-    <t>SomeScheme</t>
-  </si>
-  <si>
     <t>Version</t>
   </si>
   <si>
@@ -102,9 +206,6 @@
     <t>Hero</t>
   </si>
   <si>
-    <t>sideKick</t>
-  </si>
-  <si>
     <t>Robin</t>
   </si>
   <si>
@@ -271,13 +372,97 @@
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>Frenemies</t>
+  </si>
+  <si>
+    <t>Original Coding Scheme</t>
+  </si>
+  <si>
+    <t>LexEVS/LexGrid Elements</t>
+  </si>
+  <si>
+    <t>CodingScheme.codingSchemeName</t>
+  </si>
+  <si>
+    <t>CodingScheme.representsVersion</t>
+  </si>
+  <si>
+    <t>CodingScheme.codingSchemeURI</t>
+  </si>
+  <si>
+    <t>CodingScheme.copyright</t>
+  </si>
+  <si>
+    <t>Entity.entityCode</t>
+  </si>
+  <si>
+    <t>CodingScheme.properties.Property.propertyName = "Author"  Property.value.Text.content = "John Smith"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entity.presentationList.Presentation.propertyName = "Hero_Name" Presentation.value = "Batman" </t>
+  </si>
+  <si>
+    <t>SideKick</t>
+  </si>
+  <si>
+    <t>Sidekick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entity.commentList.Comment.propertyName = "designation" Comment.value = "Hero" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entity.propertyList.Property.propertyName = "HIstory" Property.value = "Parents Deceased" </t>
+  </si>
+  <si>
+    <t>Entity.commentList.Comment.propertyQualifierList.PropertyQualifier.propertyQualifierName = "Sidekick" PropertyQualifier.value.Text.content = "Robin"</t>
+  </si>
+  <si>
+    <t>Other Considerations:</t>
+  </si>
+  <si>
+    <t>Entity.entityCodeNamespace = "Frenimies"</t>
+  </si>
+  <si>
+    <t>Other Considerations</t>
+  </si>
+  <si>
+    <t>AssociationSource.sourceEntityCodeNamespace = "Frenimies" sourceEntityCode="001" targetList.AssociationTarget.targetEntityCodeNamespace = "Frenimies" targetEntityCode="Z41"</t>
+  </si>
+  <si>
+    <t>CodingScheme.mappings.supportedCodingSchemeList.SupportedCodingScheme.localId = "Frenimies"  uri="urn:oid:5.6.7.8"</t>
+  </si>
+  <si>
+    <t>CodingScheme.mappings.supportedNameSpaceList.SupportedNamespace.localId="Frenimies" uri="urn:oid:5.6.7.8"</t>
+  </si>
+  <si>
+    <t>CodingScheme.mappings.supportedPropertyList.SupprtedProperty.localId="Alias" propertyTypes.property uri="urn:oid:5.6.7.8"</t>
+  </si>
+  <si>
+    <t>CodingScheme.mappings.supportedPropertyQualifierList.PropertyQualifier.localId="SideKick" uri="urn:oid:5.6.7.8"</t>
+  </si>
+  <si>
+    <t>CodingScheme.mappings.supportedAssociationList.SupportedAssociation.codingScheme="Frenimies" entityCodeNamespace="Frenimies" entityCode="Z11"</t>
+  </si>
+  <si>
+    <t>CodingScheme.mappings.supportedAssociationQualifierList.SupportedAssociationQualifier.localId="restriction" uri="urn.oid:5.6.7.8"</t>
+  </si>
+  <si>
+    <t>AssociationEntity.entityCode ="Z11" forwardName="memberOf"</t>
+  </si>
+  <si>
+    <t>AssociationPredicate.associationName = "memberOf" sourceList.add(AssociationSource)</t>
+  </si>
+  <si>
+    <t>AssociationTarget.associationQualificationList.AssociationQualification.associationQualifier="restriction" qualifierText.content="current"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,13 +470,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -303,14 +536,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="10">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -642,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -657,445 +910,445 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
         <v>33</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
         <v>36</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
         <v>46</v>
-      </c>
-      <c r="C27" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1103,299 +1356,299 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C64" s="1"/>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C65" s="1"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1460,6 +1713,942 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I99"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="F9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="F10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="F11" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="F12" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="F13" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="F14" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="F15" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="F58" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="F87" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="F88" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Loader code working at a basic level. Needs review
</commit_message>
<xml_diff>
--- a/MyCodingScheme.xlsx
+++ b/MyCodingScheme.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21800" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,9 +536,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -554,15 +576,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="32">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -893,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -985,7 +1029,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>93</v>
@@ -1222,7 +1266,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1233,7 +1277,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -1244,7 +1288,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1252,7 +1296,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -1266,7 +1310,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -1277,7 +1321,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -1288,7 +1332,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1296,7 +1340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1307,7 +1351,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -1318,7 +1362,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1326,7 +1370,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -1340,7 +1384,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -1351,35 +1395,56 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
         <v>68</v>
       </c>
+      <c r="B46" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="B47" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>63</v>
+      </c>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
         <v>62</v>
       </c>
@@ -1388,56 +1453,76 @@
       </c>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="1:3">
+        <v>71</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:5">
+      <c r="A53" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="1" t="s">
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="B54" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="E54" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
@@ -1446,270 +1531,194 @@
       </c>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="1:3">
+        <v>74</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>64</v>
+      </c>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="1:3">
+        <v>75</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="1:3">
+        <v>76</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>63</v>
+      </c>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="1:3">
+        <v>77</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" s="1"/>
+      <c r="D64" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="B90" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1726,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
LEXEVS-1348, LEXEVS-1357, LEXEVS-1360.  Finished loader code base, some changes to the coding scheme source were necessary.
</commit_message>
<xml_diff>
--- a/MyCodingScheme.xlsx
+++ b/MyCodingScheme.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16020" tabRatio="500"/>
+    <workbookView xWindow="37980" yWindow="100" windowWidth="38400" windowHeight="21800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="110">
   <si>
     <t>Scheme</t>
   </si>
@@ -536,9 +536,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -576,7 +578,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="32">
+  <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -592,6 +594,7 @@
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -607,6 +610,7 @@
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -939,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1073,7 +1077,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>32</v>
@@ -1091,9 +1095,6 @@
       </c>
       <c r="C16" t="s">
         <v>30</v>
-      </c>
-      <c r="D16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1219,7 +1220,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>60</v>
@@ -1235,12 +1236,18 @@
       <c r="C29" t="s">
         <v>26</v>
       </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1290,7 +1297,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>15</v>
@@ -1350,6 +1357,9 @@
       <c r="C40" t="s">
         <v>54</v>
       </c>
+      <c r="D40" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
@@ -1364,7 +1374,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>56</v>
@@ -1654,7 +1664,7 @@
         <v>15</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>10</v>

</xml_diff>